<commit_message>
Remove zero CO2 for 2050 in the WAM emissions scenario
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_WAM_Emissions.xlsx
+++ b/SuppXLS/Scen_SYS_WAM_Emissions.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604C8DAD-90F6-451D-9708-69A111CA1E1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF301B3E-2B33-4DE4-942A-E07E647390FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4845" yWindow="4845" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
     <sheet name="config" sheetId="20" r:id="rId2"/>
     <sheet name="single" sheetId="21" r:id="rId3"/>
     <sheet name="multi" sheetId="22" r:id="rId4"/>
-    <sheet name="negative_CO2" sheetId="23" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -75,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="83">
   <si>
     <t>LimType</t>
   </si>
@@ -334,24 +333,6 @@
     <t>T-A*INT*,T-NAV*</t>
   </si>
   <si>
-    <t>~TFM_INS</t>
-  </si>
-  <si>
-    <t>TimeSlice</t>
-  </si>
-  <si>
-    <t>Attribute</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>COM_BNDNET</t>
-  </si>
-  <si>
-    <t>PWRCO2N</t>
-  </si>
-  <si>
     <t>UC_FLO</t>
   </si>
   <si>
@@ -373,7 +354,7 @@
     <numFmt numFmtId="164" formatCode="???,???.00"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,15 +451,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,18 +489,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="43"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="44"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -665,7 +627,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -687,10 +649,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="5x indented GHG Textfiels" xfId="3" xr:uid="{5F614CE9-C529-4323-B893-6D57470EC2CB}"/>
@@ -800,10 +758,6 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1894,10 +1848,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011941A8-04BF-45E8-9F60-D4E07475AB4A}">
-  <dimension ref="A1:AA17"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,14 +1859,14 @@
     <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="14" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="14" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="21" width="9.140625" style="8"/>
-    <col min="22" max="22" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="8"/>
+    <col min="4" max="13" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="20" width="9.140625" style="8"/>
+    <col min="21" max="21" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1"/>
       <c r="B1"/>
       <c r="C1"/>
@@ -1929,9 +1883,8 @@
       <c r="W1"/>
       <c r="X1"/>
       <c r="Y1"/>
-      <c r="Z1"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -1948,9 +1901,8 @@
       <c r="W2"/>
       <c r="X2"/>
       <c r="Y2"/>
-      <c r="Z2"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
@@ -1967,9 +1919,8 @@
       <c r="W3"/>
       <c r="X3"/>
       <c r="Y3"/>
-      <c r="Z3"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4" t="s">
         <v>61</v>
@@ -1990,9 +1941,8 @@
       <c r="W4"/>
       <c r="X4"/>
       <c r="Y4"/>
-      <c r="Z4"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5" t="s">
         <v>66</v>
@@ -2013,9 +1963,8 @@
       <c r="W5"/>
       <c r="X5"/>
       <c r="Y5"/>
-      <c r="Z5"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>72</v>
       </c>
@@ -2053,13 +2002,10 @@
         <v>2030</v>
       </c>
       <c r="N6" s="8">
-        <v>2050</v>
-      </c>
-      <c r="O6" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>67</v>
       </c>
@@ -2097,13 +2043,10 @@
         <v>28010</v>
       </c>
       <c r="N7" s="8">
-        <v>0</v>
-      </c>
-      <c r="O7" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>77</v>
       </c>
@@ -2147,15 +2090,11 @@
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="M8" s="8" t="str">
-        <f t="shared" ref="M8:N8" si="1">L8</f>
+        <f t="shared" ref="M8" si="1">L8</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
-      <c r="N8" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v>T-A*INT*,T-NAV*</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>62</v>
       </c>
@@ -2199,15 +2138,11 @@
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="M9" s="8" t="str">
-        <f t="shared" ref="M9:N9" si="3">L9</f>
-        <v>*CO2*,-*CO2S</v>
-      </c>
-      <c r="N9" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v>*CO2*,-*CO2S</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+        <f t="shared" ref="M9" si="3">L9</f>
+        <v>*CO2*,-*CO2S</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>71</v>
       </c>
@@ -2251,20 +2186,16 @@
         <v>ENV</v>
       </c>
       <c r="M10" s="8" t="str">
-        <f t="shared" ref="M10:N10" si="5">L10</f>
-        <v>ENV</v>
-      </c>
-      <c r="N10" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>ENV</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+        <f t="shared" ref="M10" si="5">L10</f>
+        <v>ENV</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
@@ -2308,17 +2239,13 @@
         <v>UP</v>
       </c>
       <c r="M12" s="8" t="str">
-        <f t="shared" ref="M12:N12" si="7">L12</f>
+        <f t="shared" ref="M12" si="7">L12</f>
         <v>UP</v>
       </c>
-      <c r="N12" s="8" t="str">
-        <f t="shared" si="7"/>
-        <v>UP</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C13" s="8">
         <v>-1</v>
@@ -2360,18 +2287,14 @@
         <v>-1</v>
       </c>
       <c r="M13" s="8">
-        <f t="shared" ref="M13:N13" si="9">L13</f>
+        <f t="shared" ref="M13" si="9">L13</f>
         <v>-1</v>
       </c>
-      <c r="N13" s="8">
-        <f t="shared" si="9"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C14" s="8">
         <v>1</v>
@@ -2413,13 +2336,10 @@
         <v>1</v>
       </c>
       <c r="M14" s="8">
-        <f t="shared" ref="M14:N14" si="10">L14</f>
+        <f t="shared" ref="M14" si="10">L14</f>
         <v>1</v>
       </c>
-      <c r="N14" s="8">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
+      <c r="N14"/>
       <c r="O14"/>
       <c r="P14"/>
       <c r="Q14"/>
@@ -2432,9 +2352,8 @@
       <c r="X14"/>
       <c r="Y14"/>
       <c r="Z14"/>
-      <c r="AA14"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -2451,9 +2370,8 @@
       <c r="W15"/>
       <c r="X15"/>
       <c r="Y15"/>
-      <c r="Z15"/>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -2470,9 +2388,8 @@
       <c r="W16"/>
       <c r="X16"/>
       <c r="Y16"/>
-      <c r="Z16"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -2489,7 +2406,6 @@
       <c r="W17"/>
       <c r="X17"/>
       <c r="Y17"/>
-      <c r="Z17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2499,10 +2415,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9318C9B-7F0A-410C-BCB5-F22D93E1F454}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:J31"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2563,13 +2479,13 @@
         <v>0</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>63</v>
@@ -2593,48 +2509,48 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
-        <f>VLOOKUP(B$5, config!$B$4:$O$14,2,FALSE) &amp; "_Single"</f>
+        <f>VLOOKUP(B$5, config!$B$4:$N$14,2,FALSE) &amp; "_Single"</f>
         <v>UC_NetZero_CO2_2050_Single</v>
       </c>
       <c r="C7" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F7,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F7,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F7" s="8">
         <v>2020</v>
       </c>
       <c r="G7" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F7,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H7" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F7,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J7" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F7,config!$B$6:$N$6,),FALSE)</f>
         <v>35044</v>
       </c>
       <c r="K7" s="8" t="str">
-        <f>VLOOKUP(K$5, config!$B$4:$O$14,2,FALSE) &amp; " - Single"</f>
+        <f>VLOOKUP(K$5, config!$B$4:$N$14,2,FALSE) &amp; " - Single"</f>
         <v>Net Zero CO2 by 2050 - Single</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F8,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D8" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F8,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E8" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F8,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F8" s="8">
@@ -2642,46 +2558,46 @@
         <v>2020</v>
       </c>
       <c r="I8" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F8,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F9,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D9" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F9,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F9" s="8">
         <v>2021</v>
       </c>
       <c r="G9" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F9,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H9" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F9,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J9" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F9,config!$B$6:$N$6,),FALSE)</f>
         <v>39834</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F10,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D10" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F10,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E10" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F10,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F10" s="8">
@@ -2689,46 +2605,46 @@
         <v>2021</v>
       </c>
       <c r="I10" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F10,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F11,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D11" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F11,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F11" s="8">
         <v>2022</v>
       </c>
       <c r="G11" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F11,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H11" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F11,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J11" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F11,config!$B$6:$N$6,),FALSE)</f>
         <v>38317</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F12,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D12" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F12,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E12" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F12,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F12" s="8">
@@ -2736,46 +2652,46 @@
         <v>2022</v>
       </c>
       <c r="I12" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F12,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F13,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D13" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F13,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F13" s="8">
         <v>2023</v>
       </c>
       <c r="G13" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F13,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H13" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F13,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J13" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F13,config!$B$6:$N$6,),FALSE)</f>
         <v>37424</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F14,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D14" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F14,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E14" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F14,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F14" s="8">
@@ -2783,46 +2699,46 @@
         <v>2023</v>
       </c>
       <c r="I14" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F14,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C15" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F15,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D15" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F15,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F15" s="8">
         <v>2024</v>
       </c>
       <c r="G15" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F15,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H15" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F15,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J15" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F15,config!$B$6:$N$6,),FALSE)</f>
         <v>36288</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C16" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F16,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D16" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F16,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E16" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F16,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F16" s="8">
@@ -2830,46 +2746,46 @@
         <v>2024</v>
       </c>
       <c r="I16" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F16,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F17,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D17" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F17,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F17" s="8">
         <v>2025</v>
       </c>
       <c r="G17" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F17,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H17" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F17,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J17" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F17,config!$B$6:$N$6,),FALSE)</f>
         <v>34557</v>
       </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F18,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D18" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F18,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E18" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F18,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F18" s="8">
@@ -2877,46 +2793,46 @@
         <v>2025</v>
       </c>
       <c r="I18" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F18,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F19,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D19" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F19,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F19" s="8">
         <v>2026</v>
       </c>
       <c r="G19" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F19,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H19" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F19,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J19" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F19,config!$B$6:$N$6,),FALSE)</f>
         <v>32327</v>
       </c>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F20,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D20" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F20,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E20" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F20,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F20" s="8">
@@ -2924,46 +2840,46 @@
         <v>2026</v>
       </c>
       <c r="I20" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F20,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F21,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D21" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F21,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F21" s="8">
         <v>2027</v>
       </c>
       <c r="G21" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F21,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H21" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F21,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J21" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F21,config!$B$6:$N$6,),FALSE)</f>
         <v>31553</v>
       </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F22,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D22" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F22,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E22" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F22,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F22" s="8">
@@ -2971,46 +2887,46 @@
         <v>2027</v>
       </c>
       <c r="I22" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F22,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F23,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D23" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F23,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F23" s="8">
         <v>2028</v>
       </c>
       <c r="G23" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F23,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H23" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F23,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J23" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F23,config!$B$6:$N$6,),FALSE)</f>
         <v>30410</v>
       </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F24,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D24" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F24,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E24" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F24,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F24" s="8">
@@ -3018,46 +2934,46 @@
         <v>2028</v>
       </c>
       <c r="I24" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F24,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F25,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D25" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F25,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F25" s="8">
         <v>2029</v>
       </c>
       <c r="G25" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F25,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H25" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F25,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J25" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F25,config!$B$6:$N$6,),FALSE)</f>
         <v>29410</v>
       </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F26,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D26" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F26,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E26" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F26,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F26" s="8">
@@ -3065,46 +2981,46 @@
         <v>2029</v>
       </c>
       <c r="I26" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F26,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F27,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D27" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F27,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F27" s="8">
         <v>2030</v>
       </c>
       <c r="G27" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F27,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H27" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F27,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J27" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F27,config!$B$6:$N$6,),FALSE)</f>
         <v>28010</v>
       </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F28,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D28" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F28,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E28" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F28,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F28" s="8">
@@ -3112,63 +3028,16 @@
         <v>2030</v>
       </c>
       <c r="I28" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F28,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C29" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
-        <v>*CO2*,-*CO2S</v>
-      </c>
-      <c r="D29" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
-        <v>ENV</v>
-      </c>
       <c r="F29" s="8">
-        <v>2050</v>
-      </c>
-      <c r="G29" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
-        <v>UP</v>
-      </c>
-      <c r="H29" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C30" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
-        <v>*CO2*,-*CO2S</v>
-      </c>
-      <c r="D30" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
-        <v>ENV</v>
-      </c>
-      <c r="E30" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
-        <v>T-A*INT*,T-NAV*</v>
-      </c>
-      <c r="F30" s="8">
-        <f>F29</f>
-        <v>2050</v>
-      </c>
-      <c r="I30" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F31" s="8">
-        <v>0</v>
-      </c>
-      <c r="J31" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F31,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F29,config!$B$6:$N$6,),FALSE)</f>
         <v>5</v>
       </c>
     </row>
@@ -3180,10 +3049,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EC2971-91FC-4261-B0BB-58C7F43C1746}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3244,13 +3113,13 @@
         <v>0</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>63</v>
@@ -3274,48 +3143,48 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
-        <f>VLOOKUP(B$5, config!$B$4:$O$14,2,FALSE) &amp; "_Multi"</f>
+        <f>VLOOKUP(B$5, config!$B$4:$N$14,2,FALSE) &amp; "_Multi"</f>
         <v>UC_NetZero_CO2_2050_Multi</v>
       </c>
       <c r="C7" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F7,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D7" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F7,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F7" s="8">
         <v>2020</v>
       </c>
       <c r="G7" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F7,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H7" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F7,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J7" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F7,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F7,config!$B$6:$N$6,),FALSE)</f>
         <v>35044</v>
       </c>
       <c r="K7" s="8" t="str">
-        <f>VLOOKUP(K$5, config!$B$4:$O$14,2,FALSE) &amp; " - Multi"</f>
+        <f>VLOOKUP(K$5, config!$B$4:$N$14,2,FALSE) &amp; " - Multi"</f>
         <v>Net Zero CO2 by 2050 - Multi</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F8,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D8" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F8,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E8" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F8,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F8" s="8">
@@ -3323,46 +3192,46 @@
         <v>2020</v>
       </c>
       <c r="I8" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F8,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F8,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F9,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D9" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F9,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F9" s="8">
         <v>2021</v>
       </c>
       <c r="G9" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F9,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H9" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F9,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J9" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F9,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F9,config!$B$6:$N$6,),FALSE)</f>
         <v>39834</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F10,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D10" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F10,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E10" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F10,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F10" s="8">
@@ -3370,46 +3239,46 @@
         <v>2021</v>
       </c>
       <c r="I10" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F10,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F10,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F11,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D11" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F11,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F11" s="8">
         <v>2022</v>
       </c>
       <c r="G11" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F11,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H11" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F11,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J11" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F11,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F11,config!$B$6:$N$6,),FALSE)</f>
         <v>38317</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F12,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D12" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F12,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E12" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F12,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F12" s="8">
@@ -3417,46 +3286,46 @@
         <v>2022</v>
       </c>
       <c r="I12" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F12,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F12,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F13,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D13" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F13,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F13" s="8">
         <v>2023</v>
       </c>
       <c r="G13" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F13,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H13" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F13,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J13" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F13,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F13,config!$B$6:$N$6,),FALSE)</f>
         <v>37424</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C14" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F14,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D14" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F14,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E14" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F14,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F14" s="8">
@@ -3464,46 +3333,46 @@
         <v>2023</v>
       </c>
       <c r="I14" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F14,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F14,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C15" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F15,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D15" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F15,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F15" s="8">
         <v>2024</v>
       </c>
       <c r="G15" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F15,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H15" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F15,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J15" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F15,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F15,config!$B$6:$N$6,),FALSE)</f>
         <v>36288</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C16" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F16,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D16" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F16,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E16" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F16,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F16" s="8">
@@ -3511,46 +3380,46 @@
         <v>2024</v>
       </c>
       <c r="I16" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F16,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F16,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F17,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D17" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F17,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F17" s="8">
         <v>2025</v>
       </c>
       <c r="G17" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F17,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H17" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F17,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J17" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F17,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F17,config!$B$6:$N$6,),FALSE)</f>
         <v>34557</v>
       </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F18,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D18" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F18,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E18" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F18,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F18" s="8">
@@ -3558,46 +3427,46 @@
         <v>2025</v>
       </c>
       <c r="I18" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F18,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F18,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F19,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D19" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F19,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F19" s="8">
         <v>2026</v>
       </c>
       <c r="G19" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F19,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H19" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F19,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J19" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F19,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F19,config!$B$6:$N$6,),FALSE)</f>
         <v>32327</v>
       </c>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F20,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D20" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F20,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E20" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F20,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F20" s="8">
@@ -3605,46 +3474,46 @@
         <v>2026</v>
       </c>
       <c r="I20" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F20,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F20,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F21,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D21" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F21,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F21" s="8">
         <v>2027</v>
       </c>
       <c r="G21" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F21,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H21" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F21,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J21" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F21,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F21,config!$B$6:$N$6,),FALSE)</f>
         <v>31553</v>
       </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C22" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F22,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D22" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F22,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E22" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F22,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F22" s="8">
@@ -3652,46 +3521,46 @@
         <v>2027</v>
       </c>
       <c r="I22" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F22,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F22,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F23,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D23" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F23,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F23" s="8">
         <v>2028</v>
       </c>
       <c r="G23" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F23,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H23" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F23,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J23" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F23,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F23,config!$B$6:$N$6,),FALSE)</f>
         <v>30410</v>
       </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F24,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D24" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F24,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E24" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F24,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F24" s="8">
@@ -3699,46 +3568,46 @@
         <v>2028</v>
       </c>
       <c r="I24" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F24,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F24,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F25,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D25" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F25,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F25" s="8">
         <v>2029</v>
       </c>
       <c r="G25" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F25,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H25" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F25,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J25" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F25,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F25,config!$B$6:$N$6,),FALSE)</f>
         <v>29410</v>
       </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F26,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D26" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F26,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E26" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F26,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F26" s="8">
@@ -3746,46 +3615,46 @@
         <v>2029</v>
       </c>
       <c r="I26" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F26,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F26,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F27,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D27" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F27,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="F27" s="8">
         <v>2030</v>
       </c>
       <c r="G27" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(G$5, config!$B$4:$N$14,MATCH($F27,config!$B$6:$N$6,),FALSE)</f>
         <v>UP</v>
       </c>
       <c r="H27" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(H$5, config!$B$4:$N$14,MATCH($F27,config!$B$6:$N$6,),FALSE)</f>
         <v>1</v>
       </c>
       <c r="J27" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F27,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F27,config!$B$6:$N$6,),FALSE)</f>
         <v>28010</v>
       </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F28,config!$B$6:$N$6,),FALSE)</f>
         <v>*CO2*,-*CO2S</v>
       </c>
       <c r="D28" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(D$5, config!$B$4:$N$14,MATCH($F28,config!$B$6:$N$6,),FALSE)</f>
         <v>ENV</v>
       </c>
       <c r="E28" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(E$5, config!$B$4:$N$14,MATCH($F28,config!$B$6:$N$6,),FALSE)</f>
         <v>T-A*INT*,T-NAV*</v>
       </c>
       <c r="F28" s="8">
@@ -3793,63 +3662,16 @@
         <v>2030</v>
       </c>
       <c r="I28" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F28,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP(I$5, config!$B$4:$N$14,MATCH($F28,config!$B$6:$N$6,),FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C29" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
-        <v>*CO2*,-*CO2S</v>
-      </c>
-      <c r="D29" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
-        <v>ENV</v>
-      </c>
       <c r="F29" s="8">
-        <v>2050</v>
-      </c>
-      <c r="G29" s="8" t="str">
-        <f>VLOOKUP(G$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
-        <v>UP</v>
-      </c>
-      <c r="H29" s="8">
-        <f>VLOOKUP(H$5, config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F29,config!$B$6:$O$6,),FALSE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C30" s="8" t="str">
-        <f>VLOOKUP(C$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
-        <v>*CO2*,-*CO2S</v>
-      </c>
-      <c r="D30" s="8" t="str">
-        <f>VLOOKUP(D$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
-        <v>ENV</v>
-      </c>
-      <c r="E30" s="8" t="str">
-        <f>VLOOKUP(E$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
-        <v>T-A*INT*,T-NAV*</v>
-      </c>
-      <c r="F30" s="8">
-        <f>F29</f>
-        <v>2050</v>
-      </c>
-      <c r="I30" s="8">
-        <f>VLOOKUP(I$5, config!$B$4:$O$14,MATCH($F30,config!$B$6:$O$6,),FALSE)</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="F31" s="8">
-        <v>0</v>
-      </c>
-      <c r="J31" s="8">
-        <f>VLOOKUP("Value", config!$B$4:$O$14,MATCH($F31,config!$B$6:$O$6,),FALSE)</f>
+        <f>VLOOKUP("Value", config!$B$4:$N$14,MATCH($F29,config!$B$6:$N$6,),FALSE)</f>
         <v>5</v>
       </c>
     </row>
@@ -3857,83 +3679,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2314F01-B0DB-448B-9217-DEB90E2D1CCA}">
-  <dimension ref="B2:H4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="18" t="str">
-        <f>Regions!C3</f>
-        <v>IE</v>
-      </c>
-      <c r="H3" s="18" t="str">
-        <f>Regions!D3</f>
-        <v>National</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" s="19">
-        <v>-1</v>
-      </c>
-      <c r="H4" s="19">
-        <f>G4</f>
-        <v>-1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update names of constrains to avoid overwriting
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SYS_WAM_Emissions.xlsx
+++ b/SuppXLS/Scen_SYS_WAM_Emissions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF301B3E-2B33-4DE4-942A-E07E647390FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998B644B-907E-4E94-B65D-56AA2FC95BA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -1850,8 +1850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011941A8-04BF-45E8-9F60-D4E07475AB4A}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1926,8 +1926,8 @@
         <v>61</v>
       </c>
       <c r="C4" s="8" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","NetZero","CO2","2050")</f>
-        <v>UC_NetZero_CO2_2050</v>
+        <f xml:space="preserve"> _xlfn.TEXTJOIN("_",TRUE,"UC","WAM","CO2","Emissions")</f>
+        <v>UC_WAM_CO2_Emissions</v>
       </c>
       <c r="N4"/>
       <c r="O4"/>
@@ -1948,8 +1948,8 @@
         <v>66</v>
       </c>
       <c r="C5" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"Net Zero CO2 by 2050")</f>
-        <v>Net Zero CO2 by 2050</v>
+        <f xml:space="preserve"> _xlfn.TEXTJOIN(" ",TRUE,"WAM CO2 Emissions Bound")</f>
+        <v>WAM CO2 Emissions Bound</v>
       </c>
       <c r="N5"/>
       <c r="O5"/>
@@ -2510,7 +2510,7 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
         <f>VLOOKUP(B$5, config!$B$4:$N$14,2,FALSE) &amp; "_Single"</f>
-        <v>UC_NetZero_CO2_2050_Single</v>
+        <v>UC_WAM_CO2_Emissions_Single</v>
       </c>
       <c r="C7" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F7,config!$B$6:$N$6,),FALSE)</f>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="K7" s="8" t="str">
         <f>VLOOKUP(K$5, config!$B$4:$N$14,2,FALSE) &amp; " - Single"</f>
-        <v>Net Zero CO2 by 2050 - Single</v>
+        <v>WAM CO2 Emissions Bound - Single</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3051,8 +3051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EC2971-91FC-4261-B0BB-58C7F43C1746}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3144,7 +3144,7 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
         <f>VLOOKUP(B$5, config!$B$4:$N$14,2,FALSE) &amp; "_Multi"</f>
-        <v>UC_NetZero_CO2_2050_Multi</v>
+        <v>UC_WAM_CO2_Emissions_Multi</v>
       </c>
       <c r="C7" s="8" t="str">
         <f>VLOOKUP(C$5, config!$B$4:$N$14,MATCH($F7,config!$B$6:$N$6,),FALSE)</f>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="K7" s="8" t="str">
         <f>VLOOKUP(K$5, config!$B$4:$N$14,2,FALSE) &amp; " - Multi"</f>
-        <v>Net Zero CO2 by 2050 - Multi</v>
+        <v>WAM CO2 Emissions Bound - Multi</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>